<commit_message>
THE NIR IS DEFEATED
</commit_message>
<xml_diff>
--- a/Infrared range/lista líneas infrarrojo_Benja.xlsx
+++ b/Infrared range/lista líneas infrarrojo_Benja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clauw\Documents\Programming\Final-Project\Infrared range\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E6D4EA-D194-4547-88E8-FDB91C62BD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED987BF3-0BC8-4BF1-AE2B-657295C14439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{42EE1E53-A26F-4C1C-AD90-72BD8AB225CE}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{42EE1E53-A26F-4C1C-AD90-72BD8AB225CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C157F2A4-126B-4EFE-8164-2A73FBC48E03}">
-  <dimension ref="A1:A251"/>
+  <dimension ref="A1:A246"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:XFD107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,976 +703,952 @@
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>10852.439</v>
+      <c r="A58">
+        <v>10887.245999999999</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>10887.245999999999</v>
+        <v>10899.287</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>10899.287</v>
+        <v>11610.752</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>10916.026</v>
+      <c r="A61">
+        <v>11644.987999999999</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>11610.752</v>
+        <v>11759.212</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>11644.987999999999</v>
+        <v>11786.492</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>11679.492</v>
+      <c r="A64">
+        <v>11886.099</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>11759.212</v>
+        <v>11887.338</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>11786.492</v>
+        <v>11893.744000000001</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>11886.099</v>
+      <c r="A67" s="1">
+        <v>12047.423000000001</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>11887.338</v>
+        <v>12056.382</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>11893.744000000001</v>
+        <v>12134.495000000001</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>12047.423000000001</v>
+        <v>12216.674999999999</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>12056.382</v>
+        <v>12230.459000000001</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>12134.495000000001</v>
+        <v>12286.656999999999</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
-        <v>12216.674999999999</v>
+      <c r="A73">
+        <v>12304.433000000001</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>12230.459000000001</v>
+        <v>12343.864</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>12286.656999999999</v>
+        <v>12346.290999999999</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>12304.433000000001</v>
+        <v>12413.986000000001</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>12343.864</v>
+        <v>12449.855</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>12346.290999999999</v>
+        <v>12463.174000000001</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>12413.986000000001</v>
+        <v>12479.24</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>12449.855</v>
+        <v>12513.941999999999</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>12463.174000000001</v>
+        <v>12515.671</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>12479.24</v>
+        <v>12560.433999999999</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>12513.941999999999</v>
+        <v>12619.377</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <v>12515.671</v>
+      <c r="A84" s="1">
+        <v>12642.164000000001</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>12560.433999999999</v>
+        <v>12733.441999999999</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>12619.377</v>
+        <v>12792.948</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>12642.164000000001</v>
+        <v>12810.653</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <v>12733.441999999999</v>
+      <c r="A88" s="1">
+        <v>12811.748</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <v>12792.948</v>
+      <c r="A89" s="1">
+        <v>12828.369000000001</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
-        <v>12810.653</v>
+      <c r="A90">
+        <v>12844.085999999999</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
-        <v>12811.748</v>
+      <c r="A91">
+        <v>12883.291999999999</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
-        <v>12828.369000000001</v>
+      <c r="A92">
+        <v>12899.647000000001</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>12844.085999999999</v>
+        <v>12936.543</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>12883.291999999999</v>
+        <v>13004.388000000001</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>12899.647000000001</v>
+        <v>13018.402</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>12936.543</v>
+        <v>13102.459000000001</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>13004.388000000001</v>
+        <v>13290.447</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>13018.402</v>
+        <v>13355.828</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>13102.459000000001</v>
+        <v>13395.763999999999</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>13290.447</v>
+        <v>15009.210999999999</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
-        <v>13295.421</v>
+      <c r="A101">
+        <v>15021.806</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>13355.828</v>
+        <v>15055.861999999999</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>13395.763999999999</v>
+        <v>15098.824000000001</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>15009.210999999999</v>
+        <v>15122.249</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>15021.806</v>
+        <v>15126.514999999999</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>15055.861999999999</v>
+        <v>15140.263000000001</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>15098.824000000001</v>
+        <v>15198.644</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>15122.249</v>
+        <v>15211.686</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>15126.514999999999</v>
+        <v>15223.781999999999</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>15140.263000000001</v>
+        <v>15228.891</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1">
-        <v>15188.99</v>
+      <c r="A111">
+        <v>15249.138999999999</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>15198.644</v>
+        <v>15255.175999999999</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>15211.686</v>
+        <v>15257.995000000001</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>15223.781999999999</v>
+        <v>15281.243</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>15228.891</v>
+        <v>15305.743</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>15249.138999999999</v>
+        <v>15339.578</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>15255.175999999999</v>
+        <v>15379.554</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>15257.995000000001</v>
+        <v>15431.835999999999</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>15281.243</v>
+        <v>15489.691999999999</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>15305.743</v>
+        <v>15496.377</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>15339.578</v>
+        <v>15497.789000000001</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>15379.554</v>
+        <v>15518.521000000001</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>15431.835999999999</v>
+        <v>15528.553</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>15489.691999999999</v>
+        <v>15531.454</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>15496.377</v>
+        <v>15536.003000000001</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>15497.789000000001</v>
+        <v>15538.491</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>15518.521000000001</v>
+        <v>15546.33</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>15528.553</v>
+        <v>15555.683999999999</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>15531.454</v>
+        <v>15569.485000000001</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>15536.003000000001</v>
+        <v>15570.983</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>15538.491</v>
+        <v>15575.375</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>15546.33</v>
+        <v>15575.995999999999</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>15555.683999999999</v>
+        <v>15578.317999999999</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>15569.485000000001</v>
+        <v>15583.343000000001</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>15570.983</v>
+        <v>15592.522999999999</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>15575.375</v>
+        <v>15594.31</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>15575.995999999999</v>
+        <v>15598.013000000001</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>15578.317999999999</v>
+        <v>15603.138000000001</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>15583.343000000001</v>
+        <v>15615.403</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>15592.522999999999</v>
+        <v>15625.927</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>15594.31</v>
+        <v>15636.221</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>15598.013000000001</v>
+        <v>15649.295</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>15603.138000000001</v>
+        <v>15652.790999999999</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>15615.403</v>
+        <v>15657.151</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>15625.927</v>
+        <v>15660.919</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>15636.221</v>
+        <v>15666.297</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>15649.295</v>
+        <v>15675.28</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>15652.790999999999</v>
+        <v>15686.803</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>15657.151</v>
+        <v>15696.145</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>15660.919</v>
+        <v>15727.888999999999</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>15666.297</v>
+        <v>15793.314</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>15675.28</v>
+        <v>15820.957</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>15686.803</v>
+        <v>15822.464</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>15696.145</v>
+        <v>15823.46</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>15727.888999999999</v>
+        <v>15824.757</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>15793.314</v>
+        <v>15826.035</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>15820.957</v>
+        <v>15827.144</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>15822.464</v>
+        <v>15839.491</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>15823.46</v>
+        <v>15844.522999999999</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>15824.757</v>
+        <v>15868.048000000001</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>15826.035</v>
+        <v>15868.985000000001</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>15827.144</v>
+        <v>15872.861999999999</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>15839.491</v>
+        <v>15882.787</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>15844.522999999999</v>
+        <v>15895.509</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>15868.048000000001</v>
+        <v>15899.573</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>15868.985000000001</v>
+        <v>15905.865</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>15872.861999999999</v>
+        <v>15910.39</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>15882.787</v>
+        <v>15915.652</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>15895.509</v>
+        <v>15932.52</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>15899.573</v>
+        <v>15933.83</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>15905.865</v>
+        <v>15938.375</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>15910.39</v>
+        <v>15948.207</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>15915.652</v>
+        <v>15985.093999999999</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>15932.52</v>
+        <v>16002.099</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>15933.83</v>
+        <v>16013.989</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>15938.375</v>
+        <v>16033.800999999999</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>15948.207</v>
+        <v>16045.039000000001</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>15985.093999999999</v>
+        <v>16074.575000000001</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>16002.099</v>
+        <v>16075.791999999999</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>16013.989</v>
+        <v>16080.314</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>16033.800999999999</v>
+        <v>16093.130999999999</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>16045.039000000001</v>
+        <v>16157.662</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>16074.575000000001</v>
+        <v>16160.977999999999</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>16075.791999999999</v>
+        <v>16179.397000000001</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>16080.314</v>
+        <v>16185.331</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>16093.130999999999</v>
+        <v>16199.486999999999</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>16157.662</v>
+        <v>16202.93</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>16160.977999999999</v>
+        <v>16205.945</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>16179.397000000001</v>
+        <v>16208.682000000001</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>16185.331</v>
+        <v>16212.174000000001</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>16199.486999999999</v>
+        <v>16230.056</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>16202.93</v>
+        <v>16236.088</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>16205.945</v>
+        <v>16240.404</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>16208.682000000001</v>
+        <v>16250.9</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>16212.174000000001</v>
+        <v>16263.367</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>16230.056</v>
+        <v>16276.918</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>16236.088</v>
+        <v>16281.932000000001</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>16240.404</v>
+        <v>16289.221</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>16250.9</v>
+        <v>16297.299000000001</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>16263.367</v>
+        <v>16320.782999999999</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>16276.918</v>
+        <v>16323.159</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>16281.932000000001</v>
+        <v>16328.919</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>16289.221</v>
+        <v>16335.99</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>16297.299000000001</v>
+        <v>16349.959000000001</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>16320.782999999999</v>
+        <v>16370.817999999999</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>16323.159</v>
+        <v>16388.62</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>16328.919</v>
+        <v>16398.87</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>16335.99</v>
+        <v>16409.081999999999</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>16349.959000000001</v>
+        <v>16417.463</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>16370.817999999999</v>
+        <v>16441.116000000002</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211">
-        <v>16388.62</v>
+        <v>16444.893</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>16398.87</v>
+        <v>16449.311000000002</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>16409.081999999999</v>
+        <v>16478.584999999999</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>16417.463</v>
+        <v>16491.172999999999</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>16441.116000000002</v>
+        <v>16521.740000000002</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>16444.893</v>
+        <v>16543.713</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>16449.311000000002</v>
+        <v>16556.518</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>16478.584999999999</v>
+        <v>16564.205999999998</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>16491.172999999999</v>
+        <v>16566.294000000002</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>16521.740000000002</v>
+        <v>16590.584999999999</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>16543.713</v>
+        <v>16650.423999999999</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>16556.518</v>
+        <v>16670.036</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>16564.205999999998</v>
+        <v>16683.72</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>16566.294000000002</v>
+        <v>16685.393</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>16590.584999999999</v>
+        <v>16697.64</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>16650.423999999999</v>
+        <v>16725.302</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>16670.036</v>
+        <v>16726.038</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>16683.72</v>
+        <v>16727.848000000002</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>16685.393</v>
+        <v>16729.263999999999</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>16697.64</v>
+        <v>16757.646000000001</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>16725.302</v>
+        <v>16787.624</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>16726.038</v>
+        <v>16796.811000000002</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>16727.848000000002</v>
+        <v>16798.792000000001</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>16729.263999999999</v>
+        <v>16804.240000000002</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>16757.646000000001</v>
+        <v>16847.837</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>16787.624</v>
+        <v>16868.027999999998</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>16796.811000000002</v>
+        <v>16868.663</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>16798.792000000001</v>
+        <v>16878.727999999999</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>16804.240000000002</v>
+        <v>16889.432000000001</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>16847.837</v>
+        <v>16899.798999999999</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>16868.027999999998</v>
+        <v>16903.498</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>16868.663</v>
+        <v>16933.252</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>16878.727999999999</v>
+        <v>17000.881000000001</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>16889.432000000001</v>
+        <v>17015.746999999999</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>16899.798999999999</v>
+        <v>17165.795999999998</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>16903.498</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A247">
-        <v>16933.252</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A248">
-        <v>17000.881000000001</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A249">
-        <v>17015.746999999999</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A250">
-        <v>17165.795999999998</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A251">
         <v>17170.885999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Again with the infrared range :,c
</commit_message>
<xml_diff>
--- a/Infrared range/lista líneas infrarrojo_Benja.xlsx
+++ b/Infrared range/lista líneas infrarrojo_Benja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clauw\Documents\Programming\Final-Project\Infrared range\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED987BF3-0BC8-4BF1-AE2B-657295C14439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9E439B-CE21-47E3-8DC5-19959988E19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{42EE1E53-A26F-4C1C-AD90-72BD8AB225CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{42EE1E53-A26F-4C1C-AD90-72BD8AB225CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,12 +92,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,1241 +413,1239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C157F2A4-126B-4EFE-8164-2A73FBC48E03}">
-  <dimension ref="A1:A246"/>
+  <dimension ref="A1:A245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107:XFD107"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>10022.539000000001</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>10025.035</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>10035.609</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>10060.4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>10067.804</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>10073.280000000001</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>10084.157999999999</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>10087.84</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>10089.005999999999</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10116.789000000001</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>10139.879999999999</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>10145.624</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>10148.343999999999</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>10151.86</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>10157.949000000001</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>10159.290000000001</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>10170.255999999999</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>10197.902</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>10219.114</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>10221.210999999999</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>10255.364</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+      <c r="A23" s="3">
         <v>10261.41</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>10265.276</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>10268.032999999999</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>10286.596</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>10310.279</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>10335.161</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>10343.719999999999</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>10348.019</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>10350.802</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="2">
         <v>10356.644</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="2">
         <v>10365.544</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="2">
         <v>10366.902</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>10381.846</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="2">
         <v>10391.591</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="2">
         <v>10398.646000000001</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="2">
         <v>10403.629000000001</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="2">
         <v>10404.565000000001</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="2">
         <v>10425.887000000001</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>10426.602000000001</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>10472.522999999999</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>10535.121999999999</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="2">
         <v>10558.543</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>10560.418</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>10580.039000000001</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="2">
         <v>10619.632</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+      <c r="A48" s="3">
         <v>10635.413</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>10705.976000000001</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="A50" s="2">
         <v>10724.593999999999</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="2">
         <v>10734.888999999999</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="2">
         <v>10755.953</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="A53" s="2">
         <v>10783.647000000001</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="2">
         <v>10786.004999999999</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="2">
         <v>10788.34</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>10821.24</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="2">
         <v>10836.933000000001</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="2">
         <v>10887.245999999999</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="2">
         <v>10899.287</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="2">
         <v>11610.752</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="2">
         <v>11644.987999999999</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="2">
         <v>11759.212</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="A63" s="2">
         <v>11786.492</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="A64" s="2">
         <v>11886.099</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="A65" s="2">
         <v>11887.338</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66">
+      <c r="A66" s="2">
         <v>11893.744000000001</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+      <c r="A67" s="3">
         <v>12047.423000000001</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="A68" s="2">
         <v>12056.382</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="A69" s="2">
         <v>12134.495000000001</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
+      <c r="A70" s="3">
         <v>12216.674999999999</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="A71" s="2">
         <v>12230.459000000001</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72">
+      <c r="A72" s="2">
         <v>12286.656999999999</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>12304.433000000001</v>
+      <c r="A73" s="2">
+        <v>12343.864</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <v>12343.864</v>
+      <c r="A74" s="2">
+        <v>12346.290999999999</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>12346.290999999999</v>
+      <c r="A75" s="2">
+        <v>12413.986000000001</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <v>12413.986000000001</v>
+      <c r="A76" s="2">
+        <v>12449.855</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>12449.855</v>
+      <c r="A77" s="2">
+        <v>12463.174000000001</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>12463.174000000001</v>
+      <c r="A78" s="2">
+        <v>12479.24</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>12479.24</v>
+      <c r="A79" s="2">
+        <v>12513.941999999999</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>12513.941999999999</v>
+      <c r="A80" s="2">
+        <v>12515.671</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>12515.671</v>
+      <c r="A81" s="2">
+        <v>12560.433999999999</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <v>12560.433999999999</v>
+      <c r="A82" s="2">
+        <v>12619.377</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <v>12619.377</v>
+      <c r="A83" s="3">
+        <v>12642.164000000001</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
-        <v>12642.164000000001</v>
+      <c r="A84" s="2">
+        <v>12733.441999999999</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>12733.441999999999</v>
+      <c r="A85" s="2">
+        <v>12792.948</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <v>12792.948</v>
+      <c r="A86" s="3">
+        <v>12810.653</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
-        <v>12810.653</v>
+      <c r="A87" s="3">
+        <v>12811.748</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
-        <v>12811.748</v>
+      <c r="A88" s="3">
+        <v>12828.369000000001</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
-        <v>12828.369000000001</v>
+      <c r="A89" s="2">
+        <v>12844.085999999999</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <v>12844.085999999999</v>
+      <c r="A90" s="2">
+        <v>12883.291999999999</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <v>12883.291999999999</v>
+      <c r="A91" s="2">
+        <v>12899.647000000001</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <v>12899.647000000001</v>
+      <c r="A92" s="2">
+        <v>12936.543</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <v>12936.543</v>
+      <c r="A93" s="2">
+        <v>13004.388000000001</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <v>13004.388000000001</v>
+      <c r="A94" s="2">
+        <v>13018.402</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <v>13018.402</v>
+      <c r="A95" s="2">
+        <v>13102.459000000001</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>13102.459000000001</v>
+      <c r="A96" s="2">
+        <v>13290.447</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>13290.447</v>
+      <c r="A97" s="2">
+        <v>13355.828</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>13355.828</v>
+      <c r="A98" s="2">
+        <v>13395.763999999999</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>13395.763999999999</v>
+      <c r="A99" s="2">
+        <v>15009.210999999999</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>15009.210999999999</v>
+      <c r="A100" s="2">
+        <v>15021.806</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>15021.806</v>
+      <c r="A101" s="2">
+        <v>15055.861999999999</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <v>15055.861999999999</v>
+      <c r="A102" s="2">
+        <v>15098.824000000001</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <v>15098.824000000001</v>
+      <c r="A103" s="2">
+        <v>15122.249</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <v>15122.249</v>
+      <c r="A104" s="2">
+        <v>15126.514999999999</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <v>15126.514999999999</v>
+      <c r="A105" s="2">
+        <v>15140.263000000001</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <v>15140.263000000001</v>
+      <c r="A106" s="2">
+        <v>15198.644</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <v>15198.644</v>
+      <c r="A107" s="2">
+        <v>15211.686</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <v>15211.686</v>
+      <c r="A108" s="2">
+        <v>15223.781999999999</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <v>15223.781999999999</v>
+      <c r="A109" s="2">
+        <v>15228.891</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <v>15228.891</v>
+      <c r="A110" s="2">
+        <v>15249.138999999999</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <v>15249.138999999999</v>
+      <c r="A111" s="2">
+        <v>15255.175999999999</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <v>15255.175999999999</v>
+      <c r="A112" s="2">
+        <v>15257.995000000001</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113">
-        <v>15257.995000000001</v>
+      <c r="A113" s="2">
+        <v>15281.243</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <v>15281.243</v>
+      <c r="A114" s="2">
+        <v>15305.743</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <v>15305.743</v>
+      <c r="A115" s="2">
+        <v>15339.578</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <v>15339.578</v>
+      <c r="A116" s="2">
+        <v>15379.554</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <v>15379.554</v>
+      <c r="A117" s="2">
+        <v>15431.835999999999</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <v>15431.835999999999</v>
+      <c r="A118" s="2">
+        <v>15489.691999999999</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>15489.691999999999</v>
+      <c r="A119" s="2">
+        <v>15496.377</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <v>15496.377</v>
+      <c r="A120" s="2">
+        <v>15497.789000000001</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <v>15497.789000000001</v>
+      <c r="A121" s="2">
+        <v>15518.521000000001</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <v>15518.521000000001</v>
+      <c r="A122" s="2">
+        <v>15528.553</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123">
-        <v>15528.553</v>
+      <c r="A123" s="2">
+        <v>15531.454</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <v>15531.454</v>
+      <c r="A124" s="2">
+        <v>15536.003000000001</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125">
-        <v>15536.003000000001</v>
+      <c r="A125" s="2">
+        <v>15538.491</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126">
-        <v>15538.491</v>
+      <c r="A126" s="2">
+        <v>15546.33</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127">
-        <v>15546.33</v>
+      <c r="A127" s="2">
+        <v>15555.683999999999</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128">
-        <v>15555.683999999999</v>
+      <c r="A128" s="2">
+        <v>15569.485000000001</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <v>15569.485000000001</v>
+      <c r="A129" s="2">
+        <v>15570.983</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130">
-        <v>15570.983</v>
+      <c r="A130" s="2">
+        <v>15575.375</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131">
-        <v>15575.375</v>
+      <c r="A131" s="2">
+        <v>15575.995999999999</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132">
-        <v>15575.995999999999</v>
+      <c r="A132" s="2">
+        <v>15578.317999999999</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133">
-        <v>15578.317999999999</v>
+      <c r="A133" s="2">
+        <v>15583.343000000001</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134">
-        <v>15583.343000000001</v>
+      <c r="A134" s="2">
+        <v>15592.522999999999</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135">
-        <v>15592.522999999999</v>
+      <c r="A135" s="2">
+        <v>15594.31</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136">
-        <v>15594.31</v>
+      <c r="A136" s="2">
+        <v>15598.013000000001</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137">
-        <v>15598.013000000001</v>
+      <c r="A137" s="2">
+        <v>15603.138000000001</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138">
-        <v>15603.138000000001</v>
+      <c r="A138" s="2">
+        <v>15615.403</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139">
-        <v>15615.403</v>
+      <c r="A139" s="2">
+        <v>15625.927</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140">
-        <v>15625.927</v>
+      <c r="A140" s="2">
+        <v>15636.221</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141">
-        <v>15636.221</v>
+      <c r="A141" s="2">
+        <v>15649.295</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142">
-        <v>15649.295</v>
+      <c r="A142" s="2">
+        <v>15652.790999999999</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143">
-        <v>15652.790999999999</v>
+      <c r="A143" s="2">
+        <v>15657.151</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144">
-        <v>15657.151</v>
+      <c r="A144" s="2">
+        <v>15660.919</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145">
-        <v>15660.919</v>
+      <c r="A145" s="2">
+        <v>15666.297</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146">
-        <v>15666.297</v>
+      <c r="A146" s="2">
+        <v>15675.28</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147">
-        <v>15675.28</v>
+      <c r="A147" s="2">
+        <v>15686.803</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148">
-        <v>15686.803</v>
+      <c r="A148" s="2">
+        <v>15696.145</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149">
-        <v>15696.145</v>
+      <c r="A149" s="2">
+        <v>15727.888999999999</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150">
-        <v>15727.888999999999</v>
+      <c r="A150" s="2">
+        <v>15793.314</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151">
-        <v>15793.314</v>
+      <c r="A151" s="2">
+        <v>15820.957</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152">
-        <v>15820.957</v>
+      <c r="A152" s="2">
+        <v>15822.464</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153">
-        <v>15822.464</v>
+      <c r="A153" s="2">
+        <v>15823.46</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154">
-        <v>15823.46</v>
+      <c r="A154" s="2">
+        <v>15824.757</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155">
-        <v>15824.757</v>
+      <c r="A155" s="2">
+        <v>15826.035</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156">
-        <v>15826.035</v>
+      <c r="A156" s="2">
+        <v>15827.144</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157">
-        <v>15827.144</v>
+      <c r="A157" s="2">
+        <v>15839.491</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158">
-        <v>15839.491</v>
+      <c r="A158" s="2">
+        <v>15844.522999999999</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159">
-        <v>15844.522999999999</v>
+      <c r="A159" s="2">
+        <v>15868.048000000001</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160">
-        <v>15868.048000000001</v>
+      <c r="A160" s="2">
+        <v>15868.985000000001</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161">
-        <v>15868.985000000001</v>
+      <c r="A161" s="2">
+        <v>15872.861999999999</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162">
-        <v>15872.861999999999</v>
+      <c r="A162" s="2">
+        <v>15882.787</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163">
-        <v>15882.787</v>
+      <c r="A163" s="2">
+        <v>15895.509</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164">
-        <v>15895.509</v>
+      <c r="A164" s="2">
+        <v>15899.573</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165">
-        <v>15899.573</v>
+      <c r="A165" s="2">
+        <v>15905.865</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166">
-        <v>15905.865</v>
+      <c r="A166" s="2">
+        <v>15910.39</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167">
-        <v>15910.39</v>
+      <c r="A167" s="2">
+        <v>15915.652</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168">
-        <v>15915.652</v>
+      <c r="A168" s="2">
+        <v>15932.52</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169">
-        <v>15932.52</v>
+      <c r="A169" s="2">
+        <v>15933.83</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170">
-        <v>15933.83</v>
+      <c r="A170" s="2">
+        <v>15938.375</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171">
-        <v>15938.375</v>
+      <c r="A171" s="2">
+        <v>15948.207</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172">
-        <v>15948.207</v>
+      <c r="A172" s="2">
+        <v>15985.093999999999</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173">
-        <v>15985.093999999999</v>
+      <c r="A173" s="2">
+        <v>16002.099</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174">
-        <v>16002.099</v>
+      <c r="A174" s="2">
+        <v>16013.989</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175">
-        <v>16013.989</v>
+      <c r="A175" s="2">
+        <v>16033.800999999999</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176">
-        <v>16033.800999999999</v>
+      <c r="A176" s="2">
+        <v>16045.039000000001</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177">
-        <v>16045.039000000001</v>
+      <c r="A177" s="2">
+        <v>16074.575000000001</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178">
-        <v>16074.575000000001</v>
+      <c r="A178" s="2">
+        <v>16075.791999999999</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179">
-        <v>16075.791999999999</v>
+      <c r="A179" s="2">
+        <v>16080.314</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180">
-        <v>16080.314</v>
+      <c r="A180" s="2">
+        <v>16093.130999999999</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181">
-        <v>16093.130999999999</v>
+      <c r="A181" s="2">
+        <v>16157.662</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182">
-        <v>16157.662</v>
+      <c r="A182" s="2">
+        <v>16160.977999999999</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183">
-        <v>16160.977999999999</v>
+      <c r="A183" s="2">
+        <v>16179.397000000001</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184">
-        <v>16179.397000000001</v>
+      <c r="A184" s="2">
+        <v>16185.331</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185">
-        <v>16185.331</v>
+      <c r="A185" s="2">
+        <v>16199.486999999999</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186">
-        <v>16199.486999999999</v>
+      <c r="A186" s="2">
+        <v>16202.93</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187">
-        <v>16202.93</v>
+      <c r="A187" s="2">
+        <v>16205.945</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188">
-        <v>16205.945</v>
+      <c r="A188" s="2">
+        <v>16208.682000000001</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189">
-        <v>16208.682000000001</v>
+      <c r="A189" s="2">
+        <v>16212.174000000001</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190">
-        <v>16212.174000000001</v>
+      <c r="A190" s="2">
+        <v>16230.056</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191">
-        <v>16230.056</v>
+      <c r="A191" s="2">
+        <v>16236.088</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192">
-        <v>16236.088</v>
+      <c r="A192" s="2">
+        <v>16240.404</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193">
-        <v>16240.404</v>
+      <c r="A193" s="2">
+        <v>16250.9</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194">
-        <v>16250.9</v>
+      <c r="A194" s="2">
+        <v>16263.367</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195">
-        <v>16263.367</v>
+      <c r="A195" s="2">
+        <v>16276.918</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196">
-        <v>16276.918</v>
+      <c r="A196" s="2">
+        <v>16281.932000000001</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197">
-        <v>16281.932000000001</v>
+      <c r="A197" s="2">
+        <v>16289.221</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A198">
-        <v>16289.221</v>
+      <c r="A198" s="2">
+        <v>16297.299000000001</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A199">
-        <v>16297.299000000001</v>
+      <c r="A199" s="2">
+        <v>16320.782999999999</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A200">
-        <v>16320.782999999999</v>
+      <c r="A200" s="2">
+        <v>16323.159</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A201">
-        <v>16323.159</v>
+      <c r="A201" s="2">
+        <v>16328.919</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A202">
-        <v>16328.919</v>
+      <c r="A202" s="2">
+        <v>16335.99</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A203">
-        <v>16335.99</v>
+      <c r="A203" s="2">
+        <v>16349.959000000001</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A204">
-        <v>16349.959000000001</v>
+      <c r="A204" s="2">
+        <v>16370.817999999999</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A205">
-        <v>16370.817999999999</v>
+      <c r="A205" s="2">
+        <v>16388.62</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A206">
-        <v>16388.62</v>
+      <c r="A206" s="2">
+        <v>16398.87</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A207">
-        <v>16398.87</v>
+      <c r="A207" s="2">
+        <v>16409.081999999999</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A208">
-        <v>16409.081999999999</v>
+      <c r="A208" s="2">
+        <v>16417.463</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A209">
-        <v>16417.463</v>
+      <c r="A209" s="2">
+        <v>16441.116000000002</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A210">
-        <v>16441.116000000002</v>
+      <c r="A210" s="2">
+        <v>16444.893</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A211">
-        <v>16444.893</v>
+      <c r="A211" s="2">
+        <v>16449.311000000002</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A212">
-        <v>16449.311000000002</v>
+      <c r="A212" s="2">
+        <v>16478.584999999999</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A213">
-        <v>16478.584999999999</v>
+      <c r="A213" s="2">
+        <v>16491.172999999999</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A214">
-        <v>16491.172999999999</v>
+      <c r="A214" s="2">
+        <v>16521.740000000002</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A215">
-        <v>16521.740000000002</v>
+      <c r="A215" s="2">
+        <v>16543.713</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A216">
-        <v>16543.713</v>
+      <c r="A216" s="2">
+        <v>16556.518</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A217">
-        <v>16556.518</v>
+      <c r="A217" s="2">
+        <v>16564.205999999998</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A218">
-        <v>16564.205999999998</v>
+      <c r="A218" s="2">
+        <v>16566.294000000002</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A219">
-        <v>16566.294000000002</v>
+      <c r="A219" s="2">
+        <v>16590.584999999999</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A220">
-        <v>16590.584999999999</v>
+      <c r="A220" s="2">
+        <v>16650.423999999999</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A221">
-        <v>16650.423999999999</v>
+      <c r="A221" s="2">
+        <v>16670.036</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A222">
-        <v>16670.036</v>
+      <c r="A222" s="2">
+        <v>16683.72</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A223">
-        <v>16683.72</v>
+      <c r="A223" s="2">
+        <v>16685.393</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A224">
-        <v>16685.393</v>
+      <c r="A224" s="2">
+        <v>16697.64</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A225">
-        <v>16697.64</v>
+      <c r="A225" s="2">
+        <v>16725.302</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A226">
-        <v>16725.302</v>
+      <c r="A226" s="2">
+        <v>16726.038</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A227">
-        <v>16726.038</v>
+      <c r="A227" s="2">
+        <v>16727.848000000002</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A228">
-        <v>16727.848000000002</v>
+      <c r="A228" s="2">
+        <v>16729.263999999999</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A229">
-        <v>16729.263999999999</v>
+      <c r="A229" s="2">
+        <v>16757.646000000001</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A230">
-        <v>16757.646000000001</v>
+      <c r="A230" s="2">
+        <v>16787.624</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A231">
-        <v>16787.624</v>
+      <c r="A231" s="2">
+        <v>16796.811000000002</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A232">
-        <v>16796.811000000002</v>
+      <c r="A232" s="2">
+        <v>16798.792000000001</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A233">
-        <v>16798.792000000001</v>
+      <c r="A233" s="2">
+        <v>16804.240000000002</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A234">
-        <v>16804.240000000002</v>
+      <c r="A234" s="2">
+        <v>16847.837</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A235">
-        <v>16847.837</v>
+      <c r="A235" s="2">
+        <v>16868.027999999998</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A236">
-        <v>16868.027999999998</v>
+      <c r="A236" s="2">
+        <v>16868.663</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A237">
-        <v>16868.663</v>
+      <c r="A237" s="2">
+        <v>16878.727999999999</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A238">
-        <v>16878.727999999999</v>
+      <c r="A238" s="2">
+        <v>16889.432000000001</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A239">
-        <v>16889.432000000001</v>
+      <c r="A239" s="2">
+        <v>16899.798999999999</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A240">
-        <v>16899.798999999999</v>
+      <c r="A240" s="2">
+        <v>16903.498</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A241">
-        <v>16903.498</v>
+      <c r="A241" s="2">
+        <v>16933.252</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A242">
-        <v>16933.252</v>
+      <c r="A242" s="2">
+        <v>17000.881000000001</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A243">
-        <v>17000.881000000001</v>
+      <c r="A243" s="2">
+        <v>17015.746999999999</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A244">
-        <v>17015.746999999999</v>
+      <c r="A244" s="2">
+        <v>17165.795999999998</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A245">
-        <v>17165.795999999998</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A246">
+      <c r="A245" s="2">
         <v>17170.885999999999</v>
       </c>
     </row>

</xml_diff>